<commit_message>
extend cache conflict benchmark to exhaust l3 cache
</commit_message>
<xml_diff>
--- a/lecture_01/results.xlsx
+++ b/lecture_01/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="279">
   <si>
     <t>Run on (8 X 4008 MHz CPU s)</t>
   </si>
@@ -843,6 +843,24 @@
   </si>
   <si>
     <t>BM_cache_conflict/3/0</t>
+  </si>
+  <si>
+    <t>BM_cache_conflict/11/1</t>
+  </si>
+  <si>
+    <t>BM_cache_conflict/12/1</t>
+  </si>
+  <si>
+    <t>BM_cache_conflict/13/1</t>
+  </si>
+  <si>
+    <t>BM_cache_conflict/11/0</t>
+  </si>
+  <si>
+    <t>BM_cache_conflict/12/0</t>
+  </si>
+  <si>
+    <t>BM_cache_conflict/13/0</t>
   </si>
 </sst>
 </file>
@@ -3366,10 +3384,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>cc_plot!$A$2:$A$12</c:f>
+              <c:f>cc_plot!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3402,18 +3420,27 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>cc_plot!$B$2:$B$12</c:f>
+              <c:f>cc_plot!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.3392900000000001</c:v>
+                  <c:v>1.31836</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.6113299999999999</c:v>
@@ -3425,13 +3452,13 @@
                   <c:v>1.5346</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8223374999999999</c:v>
+                  <c:v>1.80489375</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.66015625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7874531250000001</c:v>
+                  <c:v>1.8746562499999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.5558437500000002</c:v>
@@ -3444,6 +3471,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5.18798828125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.05517578125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.3514404296875</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.7091064453125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3495,10 +3531,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>cc_plot!$A$2:$A$12</c:f>
+              <c:f>cc_plot!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3531,48 +3567,66 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>cc_plot!$C$2:$C$12</c:f>
+              <c:f>cc_plot!$C$2:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>1.3392900000000001</c:v>
+                  <c:v>1.31138</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.569475</c:v>
+                  <c:v>1.604355</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1.569475</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5346</c:v>
+                  <c:v>1.569475</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3018999999999998</c:v>
+                  <c:v>2.3062562500000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2.6702875000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1171562499999999</c:v>
+                  <c:v>3.0463125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.463203125</c:v>
+                  <c:v>10.245156250000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.544921875</c:v>
+                  <c:v>11.035351562500001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.68115234375</c:v>
+                  <c:v>10.986328125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.96728515625</c:v>
+                  <c:v>11.68251953125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.4140625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>57.220458984375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.9425048828125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21344,10 +21398,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection sqref="A1:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21359,7 +21413,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43028.122812499998</v>
+        <v>43028.162870370368</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -21405,13 +21459,13 @@
         <v>265</v>
       </c>
       <c r="B4">
-        <v>560000000</v>
+        <v>497777778</v>
       </c>
       <c r="C4">
-        <v>1.32626</v>
+        <v>1.3259799999999999</v>
       </c>
       <c r="D4">
-        <v>1.3392900000000001</v>
+        <v>1.31836</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -21431,7 +21485,7 @@
         <v>213333333</v>
       </c>
       <c r="C5">
-        <v>3.19475</v>
+        <v>3.2218100000000001</v>
       </c>
       <c r="D5">
         <v>3.2226599999999999</v>
@@ -21454,7 +21508,7 @@
         <v>112000000</v>
       </c>
       <c r="C6">
-        <v>6.1871600000000004</v>
+        <v>6.1873300000000002</v>
       </c>
       <c r="D6">
         <v>6.1383900000000002</v>
@@ -21477,7 +21531,7 @@
         <v>56000000</v>
       </c>
       <c r="C7">
-        <v>12.3728</v>
+        <v>12.3729</v>
       </c>
       <c r="D7">
         <v>12.2768</v>
@@ -21497,13 +21551,13 @@
         <v>248</v>
       </c>
       <c r="B8">
-        <v>23578947</v>
+        <v>24888889</v>
       </c>
       <c r="C8">
-        <v>29.2012</v>
+        <v>29.255299999999998</v>
       </c>
       <c r="D8">
-        <v>29.157399999999999</v>
+        <v>28.878299999999999</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -21523,7 +21577,7 @@
         <v>10000000</v>
       </c>
       <c r="C9">
-        <v>52.872100000000003</v>
+        <v>52.867400000000004</v>
       </c>
       <c r="D9">
         <v>53.125</v>
@@ -21546,10 +21600,10 @@
         <v>5600000</v>
       </c>
       <c r="C10">
-        <v>113.878</v>
+        <v>119.119</v>
       </c>
       <c r="D10">
-        <v>114.39700000000001</v>
+        <v>119.97799999999999</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -21569,7 +21623,7 @@
         <v>1544828</v>
       </c>
       <c r="C11">
-        <v>455.37400000000002</v>
+        <v>455.32299999999998</v>
       </c>
       <c r="D11">
         <v>455.14800000000002</v>
@@ -21592,7 +21646,7 @@
         <v>746667</v>
       </c>
       <c r="C12">
-        <v>936.20299999999997</v>
+        <v>936.45799999999997</v>
       </c>
       <c r="D12">
         <v>941.68499999999995</v>
@@ -21615,7 +21669,7 @@
         <v>373333</v>
       </c>
       <c r="C13">
-        <v>1925.09</v>
+        <v>1922.39</v>
       </c>
       <c r="D13">
         <v>1925.22</v>
@@ -21638,7 +21692,7 @@
         <v>100000</v>
       </c>
       <c r="C14">
-        <v>5396.53</v>
+        <v>5397.44</v>
       </c>
       <c r="D14">
         <v>5312.5</v>
@@ -21655,85 +21709,85 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B15">
-        <v>560000000</v>
+        <v>40727</v>
       </c>
       <c r="C15">
-        <v>1.32596</v>
+        <v>16368.6</v>
       </c>
       <c r="D15">
-        <v>1.3392900000000001</v>
+        <v>16497</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B16">
-        <v>224000000</v>
+        <v>10000</v>
       </c>
       <c r="C16">
-        <v>3.1273200000000001</v>
+        <v>55459.9</v>
       </c>
       <c r="D16">
-        <v>3.1389499999999999</v>
+        <v>54687.5</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B17">
-        <v>112000000</v>
+        <v>6400</v>
       </c>
       <c r="C17">
-        <v>6.1871999999999998</v>
+        <v>110953</v>
       </c>
       <c r="D17">
-        <v>6.2778999999999998</v>
+        <v>112305</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B18">
-        <v>56000000</v>
+        <v>560000000</v>
       </c>
       <c r="C18">
-        <v>12.374599999999999</v>
+        <v>1.32623</v>
       </c>
       <c r="D18">
-        <v>12.2768</v>
+        <v>1.31138</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
@@ -21742,21 +21796,21 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B19">
-        <v>18666667</v>
+        <v>224000000</v>
       </c>
       <c r="C19">
-        <v>36.679499999999997</v>
+        <v>3.2066699999999999</v>
       </c>
       <c r="D19">
-        <v>36.830399999999997</v>
+        <v>3.20871</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -21765,21 +21819,21 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="B20">
-        <v>8960000</v>
+        <v>112000000</v>
       </c>
       <c r="C20">
-        <v>85.716999999999999</v>
+        <v>6.1869399999999999</v>
       </c>
       <c r="D20">
-        <v>85.449200000000005</v>
+        <v>6.2778999999999998</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -21788,21 +21842,21 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="B21">
-        <v>3446154</v>
+        <v>56000000</v>
       </c>
       <c r="C21">
-        <v>195.94900000000001</v>
+        <v>12.372400000000001</v>
       </c>
       <c r="D21">
-        <v>199.49799999999999</v>
+        <v>12.5558</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -21811,21 +21865,21 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B22">
-        <v>560000</v>
+        <v>19478261</v>
       </c>
       <c r="C22">
-        <v>1325.75</v>
+        <v>36.692100000000003</v>
       </c>
       <c r="D22">
-        <v>1339.29</v>
+        <v>36.900100000000002</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -21834,21 +21888,21 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B23">
-        <v>248889</v>
+        <v>8960000</v>
       </c>
       <c r="C23">
-        <v>2734.6</v>
+        <v>85.726399999999998</v>
       </c>
       <c r="D23">
-        <v>2699.5</v>
+        <v>85.449200000000005</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -21857,21 +21911,21 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B24">
-        <v>100000</v>
+        <v>3446154</v>
       </c>
       <c r="C24">
-        <v>5576.98</v>
+        <v>195.74700000000001</v>
       </c>
       <c r="D24">
-        <v>5468.75</v>
+        <v>194.964</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -21880,21 +21934,21 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B25">
-        <v>64000</v>
+        <v>560000</v>
       </c>
       <c r="C25">
-        <v>11247.3</v>
+        <v>1313.22</v>
       </c>
       <c r="D25">
-        <v>11230.5</v>
+        <v>1311.38</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -21903,7 +21957,145 @@
         <v>0</v>
       </c>
       <c r="L25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26">
+        <v>248889</v>
+      </c>
+      <c r="C26">
+        <v>2797.74</v>
+      </c>
+      <c r="D26">
+        <v>2825.05</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27">
+        <v>100000</v>
+      </c>
+      <c r="C27">
+        <v>5698.97</v>
+      </c>
+      <c r="D27">
+        <v>5625</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B28">
+        <v>64000</v>
+      </c>
+      <c r="C28">
+        <v>12011.7</v>
+      </c>
+      <c r="D28">
+        <v>11962.9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
         <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>276</v>
+      </c>
+      <c r="B29">
+        <v>10000</v>
+      </c>
+      <c r="C29">
+        <v>49537.1</v>
+      </c>
+      <c r="D29">
+        <v>50000</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30">
+        <v>3200</v>
+      </c>
+      <c r="C30">
+        <v>235429</v>
+      </c>
+      <c r="D30">
+        <v>234375</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31">
+        <v>1000</v>
+      </c>
+      <c r="C31">
+        <v>505277</v>
+      </c>
+      <c r="D31">
+        <v>515625</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -21913,10 +22105,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21959,7 +22151,7 @@
       </c>
       <c r="C2">
         <f>cc_results!D4</f>
-        <v>1.3392900000000001</v>
+        <v>1.31836</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("2^",B2)</f>
@@ -21967,7 +22159,7 @@
       </c>
       <c r="E2">
         <f>C2/2^B2</f>
-        <v>1.3392900000000001</v>
+        <v>1.31836</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -22047,7 +22239,7 @@
       </c>
       <c r="C6">
         <f>cc_results!D8</f>
-        <v>29.157399999999999</v>
+        <v>28.878299999999999</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -22055,7 +22247,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>1.8223374999999999</v>
+        <v>1.80489375</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -22091,7 +22283,7 @@
       </c>
       <c r="C8">
         <f>cc_results!D10</f>
-        <v>114.39700000000001</v>
+        <v>119.97799999999999</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -22099,7 +22291,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>1.7874531250000001</v>
+        <v>1.8746562499999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -22193,67 +22385,67 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CHOOSE(cc_results!K15 + 1,"aligned","unaligned")</f>
-        <v>aligned</v>
+        <v>unaligned</v>
       </c>
       <c r="B13">
         <f>cc_results!L15</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <f>cc_results!D15</f>
-        <v>1.3392900000000001</v>
+        <v>16497</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>2^0</v>
+        <v>2^11</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>1.3392900000000001</v>
+        <v>8.05517578125</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CHOOSE(cc_results!K16 + 1,"aligned","unaligned")</f>
-        <v>aligned</v>
+        <v>unaligned</v>
       </c>
       <c r="B14">
         <f>cc_results!L16</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <f>cc_results!D16</f>
-        <v>3.1389499999999999</v>
+        <v>54687.5</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>2^1</v>
+        <v>2^12</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>1.569475</v>
+        <v>13.3514404296875</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CHOOSE(cc_results!K17 + 1,"aligned","unaligned")</f>
-        <v>aligned</v>
+        <v>unaligned</v>
       </c>
       <c r="B15">
         <f>cc_results!L17</f>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C15">
         <f>cc_results!D17</f>
-        <v>6.2778999999999998</v>
+        <v>112305</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>2^2</v>
+        <v>2^13</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>1.569475</v>
+        <v>13.7091064453125</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -22263,19 +22455,19 @@
       </c>
       <c r="B16">
         <f>cc_results!L18</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <f>cc_results!D18</f>
-        <v>12.2768</v>
+        <v>1.31138</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ref="D16:D31" si="2">CONCATENATE("2^",B16)</f>
-        <v>2^3</v>
+        <v>2^0</v>
       </c>
       <c r="E16">
         <f t="shared" ref="E16:E31" si="3">C16/2^B16</f>
-        <v>1.5346</v>
+        <v>1.31138</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -22285,19 +22477,19 @@
       </c>
       <c r="B17">
         <f>cc_results!L19</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <f>cc_results!D19</f>
-        <v>36.830399999999997</v>
+        <v>3.20871</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="2"/>
-        <v>2^4</v>
+        <v>2^1</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>2.3018999999999998</v>
+        <v>1.604355</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -22307,19 +22499,19 @@
       </c>
       <c r="B18">
         <f>cc_results!L20</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <f>cc_results!D20</f>
-        <v>85.449200000000005</v>
+        <v>6.2778999999999998</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="2"/>
-        <v>2^5</v>
+        <v>2^2</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>2.6702875000000001</v>
+        <v>1.569475</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -22329,19 +22521,19 @@
       </c>
       <c r="B19">
         <f>cc_results!L21</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <f>cc_results!D21</f>
-        <v>199.49799999999999</v>
+        <v>12.5558</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="2"/>
-        <v>2^6</v>
+        <v>2^3</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>3.1171562499999999</v>
+        <v>1.569475</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -22351,19 +22543,19 @@
       </c>
       <c r="B20">
         <f>cc_results!L22</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C20">
         <f>cc_results!D22</f>
-        <v>1339.29</v>
+        <v>36.900100000000002</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="2"/>
-        <v>2^7</v>
+        <v>2^4</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>10.463203125</v>
+        <v>2.3062562500000001</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -22373,19 +22565,19 @@
       </c>
       <c r="B21">
         <f>cc_results!L23</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <f>cc_results!D23</f>
-        <v>2699.5</v>
+        <v>85.449200000000005</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="2"/>
-        <v>2^8</v>
+        <v>2^5</v>
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
-        <v>10.544921875</v>
+        <v>2.6702875000000001</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -22395,19 +22587,19 @@
       </c>
       <c r="B22">
         <f>cc_results!L24</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <f>cc_results!D24</f>
-        <v>5468.75</v>
+        <v>194.964</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="2"/>
-        <v>2^9</v>
+        <v>2^6</v>
       </c>
       <c r="E22">
         <f t="shared" si="3"/>
-        <v>10.68115234375</v>
+        <v>3.0463125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -22417,19 +22609,151 @@
       </c>
       <c r="B23">
         <f>cc_results!L25</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <f>cc_results!D25</f>
-        <v>11230.5</v>
+        <v>1311.38</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="2"/>
-        <v>2^10</v>
+        <v>2^7</v>
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
-        <v>10.96728515625</v>
+        <v>10.245156250000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>CHOOSE(cc_results!K26 + 1,"aligned","unaligned")</f>
+        <v>aligned</v>
+      </c>
+      <c r="B24">
+        <f>cc_results!L26</f>
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <f>cc_results!D26</f>
+        <v>2825.05</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" ref="D24:D31" si="4">CONCATENATE("2^",B24)</f>
+        <v>2^8</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E24:E31" si="5">C24/2^B24</f>
+        <v>11.035351562500001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>CHOOSE(cc_results!K27 + 1,"aligned","unaligned")</f>
+        <v>aligned</v>
+      </c>
+      <c r="B25">
+        <f>cc_results!L27</f>
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <f>cc_results!D27</f>
+        <v>5625</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="4"/>
+        <v>2^9</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="5"/>
+        <v>10.986328125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>CHOOSE(cc_results!K28 + 1,"aligned","unaligned")</f>
+        <v>aligned</v>
+      </c>
+      <c r="B26">
+        <f>cc_results!L28</f>
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <f>cc_results!D28</f>
+        <v>11962.9</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="4"/>
+        <v>2^10</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="5"/>
+        <v>11.68251953125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>CHOOSE(cc_results!K29 + 1,"aligned","unaligned")</f>
+        <v>aligned</v>
+      </c>
+      <c r="B27">
+        <f>cc_results!L29</f>
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <f>cc_results!D29</f>
+        <v>50000</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="4"/>
+        <v>2^11</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>24.4140625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>CHOOSE(cc_results!K30 + 1,"aligned","unaligned")</f>
+        <v>aligned</v>
+      </c>
+      <c r="B28">
+        <f>cc_results!L30</f>
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <f>cc_results!D30</f>
+        <v>234375</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="4"/>
+        <v>2^12</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="5"/>
+        <v>57.220458984375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>CHOOSE(cc_results!K31 + 1,"aligned","unaligned")</f>
+        <v>aligned</v>
+      </c>
+      <c r="B29">
+        <f>cc_results!L31</f>
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <f>cc_results!D31</f>
+        <v>515625</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="4"/>
+        <v>2^13</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="5"/>
+        <v>62.9425048828125</v>
       </c>
     </row>
   </sheetData>
@@ -22439,10 +22763,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="AD22" sqref="AD22"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22461,7 +22785,7 @@
         <v>unaligned</v>
       </c>
       <c r="C1" t="str">
-        <f>cc_charts!A13</f>
+        <f>cc_charts!A16</f>
         <v>aligned</v>
       </c>
     </row>
@@ -22472,11 +22796,11 @@
       </c>
       <c r="B2">
         <f>cc_charts!E2</f>
-        <v>1.3392900000000001</v>
+        <v>1.31836</v>
       </c>
       <c r="C2">
-        <f>cc_charts!E13</f>
-        <v>1.3392900000000001</v>
+        <f>cc_charts!E16</f>
+        <v>1.31138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -22489,8 +22813,8 @@
         <v>1.6113299999999999</v>
       </c>
       <c r="C3">
-        <f>cc_charts!E14</f>
-        <v>1.569475</v>
+        <f>cc_charts!E17</f>
+        <v>1.604355</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -22503,7 +22827,7 @@
         <v>1.5345975000000001</v>
       </c>
       <c r="C4">
-        <f>cc_charts!E15</f>
+        <f>cc_charts!E18</f>
         <v>1.569475</v>
       </c>
     </row>
@@ -22517,8 +22841,8 @@
         <v>1.5346</v>
       </c>
       <c r="C5">
-        <f>cc_charts!E16</f>
-        <v>1.5346</v>
+        <f>cc_charts!E19</f>
+        <v>1.569475</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -22528,11 +22852,11 @@
       </c>
       <c r="B6">
         <f>cc_charts!E6</f>
-        <v>1.8223374999999999</v>
+        <v>1.80489375</v>
       </c>
       <c r="C6">
-        <f>cc_charts!E17</f>
-        <v>2.3018999999999998</v>
+        <f>cc_charts!E20</f>
+        <v>2.3062562500000001</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -22545,7 +22869,7 @@
         <v>1.66015625</v>
       </c>
       <c r="C7">
-        <f>cc_charts!E18</f>
+        <f>cc_charts!E21</f>
         <v>2.6702875000000001</v>
       </c>
     </row>
@@ -22556,11 +22880,11 @@
       </c>
       <c r="B8">
         <f>cc_charts!E8</f>
-        <v>1.7874531250000001</v>
+        <v>1.8746562499999999</v>
       </c>
       <c r="C8">
-        <f>cc_charts!E19</f>
-        <v>3.1171562499999999</v>
+        <f>cc_charts!E22</f>
+        <v>3.0463125</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -22573,8 +22897,8 @@
         <v>3.5558437500000002</v>
       </c>
       <c r="C9">
-        <f>cc_charts!E20</f>
-        <v>10.463203125</v>
+        <f>cc_charts!E23</f>
+        <v>10.245156250000001</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -22587,8 +22911,8 @@
         <v>3.6784570312499998</v>
       </c>
       <c r="C10">
-        <f>cc_charts!E21</f>
-        <v>10.544921875</v>
+        <f>cc_charts!E24</f>
+        <v>11.035351562500001</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -22601,8 +22925,8 @@
         <v>3.7601953125000001</v>
       </c>
       <c r="C11">
-        <f>cc_charts!E22</f>
-        <v>10.68115234375</v>
+        <f>cc_charts!E25</f>
+        <v>10.986328125</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -22615,8 +22939,50 @@
         <v>5.18798828125</v>
       </c>
       <c r="C12">
-        <f>cc_charts!E23</f>
-        <v>10.96728515625</v>
+        <f>cc_charts!E26</f>
+        <v>11.68251953125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>2^cc_charts!B13</f>
+        <v>2048</v>
+      </c>
+      <c r="B13">
+        <f>cc_charts!E13</f>
+        <v>8.05517578125</v>
+      </c>
+      <c r="C13">
+        <f>cc_charts!E27</f>
+        <v>24.4140625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>2^cc_charts!B14</f>
+        <v>4096</v>
+      </c>
+      <c r="B14">
+        <f>cc_charts!E14</f>
+        <v>13.3514404296875</v>
+      </c>
+      <c r="C14">
+        <f>cc_charts!E28</f>
+        <v>57.220458984375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>2^cc_charts!B15</f>
+        <v>8192</v>
+      </c>
+      <c r="B15">
+        <f>cc_charts!E15</f>
+        <v>13.7091064453125</v>
+      </c>
+      <c r="C15">
+        <f>cc_charts!E29</f>
+        <v>62.9425048828125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>